<commit_message>
new function - reading project info from xlsx
</commit_message>
<xml_diff>
--- a/projekt_info.xlsx
+++ b/projekt_info.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\github\test_github\PythonPaintProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858668C3-3FC9-4375-B8CE-B96EB7B5A5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8312C0-E7F2-4E56-A304-8D902250D016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arbeitsschritte" sheetId="1" r:id="rId1"/>
+    <sheet name="Projekt" sheetId="2" r:id="rId1"/>
+    <sheet name="Arbeitsschritte" sheetId="1" r:id="rId2"/>
+    <sheet name="Bauabschnitte" sheetId="3" r:id="rId3"/>
+    <sheet name="Hilfstabelle" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Beton</t>
   </si>
@@ -58,13 +61,175 @@
   </si>
   <si>
     <t>Arbeitsschritte</t>
+  </si>
+  <si>
+    <t>Projektname</t>
+  </si>
+  <si>
+    <t>Bundesland</t>
+  </si>
+  <si>
+    <t>Arbeiten am Samstag [ja/nein]</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>BYP</t>
+  </si>
+  <si>
+    <t>HB</t>
+  </si>
+  <si>
+    <t>HE</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Anzahl der Bauabschnitte</t>
+  </si>
+  <si>
+    <t>[ja/nein]</t>
+  </si>
+  <si>
+    <t>nein</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +250,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +315,186 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8057FF"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF696969"/>
+        <bgColor rgb="FF696969"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB03060"/>
+        <bgColor rgb="FFB03060"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF006400"/>
+        <bgColor rgb="FF006400"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808000"/>
+        <bgColor rgb="FF808000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF483D8B"/>
+        <bgColor rgb="FF483D8B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008B8B"/>
+        <bgColor rgb="FF008B8B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000080"/>
+        <bgColor rgb="FF000080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD2691E"/>
+        <bgColor rgb="FFD2691E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9ACD32"/>
+        <bgColor rgb="FF9ACD32"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FBC8F"/>
+        <bgColor rgb="FF8FBC8F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8B008B"/>
+        <bgColor rgb="FF8B008B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCD2990"/>
+        <bgColor rgb="FFCD2990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4500"/>
+        <bgColor rgb="FFFF4500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+        <bgColor rgb="FFFFA500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7CFC00"/>
+        <bgColor rgb="FF7CFC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8A2BE2"/>
+        <bgColor rgb="FF8A2BE2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF7F"/>
+        <bgColor rgb="FF00FF7F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9967A"/>
+        <bgColor rgb="FFE9967A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDC143C"/>
+        <bgColor rgb="FFDC143C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00BFFF"/>
+        <bgColor rgb="FF00BFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB0C4DE"/>
+        <bgColor rgb="FFB0C4DE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1E90FF"/>
+        <bgColor rgb="FF1E90FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDA0DD"/>
+        <bgColor rgb="FFDDA0DD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90EE90"/>
+        <bgColor rgb="FF90EE90"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF1493"/>
+        <bgColor rgb="FFFF1493"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE4C4"/>
+        <bgColor rgb="FFFFE4C4"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -172,6 +522,39 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -464,17 +847,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5D15DC-0F6E-4BF4-B870-E676A4C2C0FF}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C11AAA84-D484-4056-A415-81156A811647}">
+          <x14:formula1>
+            <xm:f>Hilfstabelle!$A$2:$A$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{64A133BD-5DD1-4968-BE7D-4694599E4E4D}">
+          <x14:formula1>
+            <xm:f>Hilfstabelle!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -482,7 +932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -504,7 +954,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -518,7 +968,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -544,4 +994,284 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22201E99-7EBB-46A1-8838-B06109ACFC34}">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEEEA13-DE67-41F2-9AFC-D4F8D7A0E2C4}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>